<commit_message>
Updates to assay spreadsheet template to support named SNPs and ROIs
</commit_message>
<xml_diff>
--- a/assay_data/LymeSeq_assays.xlsx
+++ b/assay_data/LymeSeq_assays.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16760" yWindow="5680" windowWidth="34600" windowHeight="21700" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="6260" windowWidth="34600" windowHeight="21700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LymeSeq_1608" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="255">
   <si>
     <t>Assay Name</t>
   </si>
@@ -979,12 +979,53 @@
   <si>
     <t>references/rrs-rrlA_amplicons_derep_group.fasta</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Positions</t>
+  </si>
+  <si>
+    <r>
+      <t>AA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/NT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sequence</t>
+    </r>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1102,7 +1143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1223,450 +1264,489 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="421">
+  <cellStyleXfs count="427">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
@@ -1677,11 +1757,11 @@
       <alignment horizontal="fill"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1692,7 +1772,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1706,8 +1786,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="50" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1720,48 +1800,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="50" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="420" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="420" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="421">
+  <cellStyles count="427">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2104,6 +2196,9 @@
     <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2179,6 +2274,9 @@
     <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="50" builtinId="10"/>
     <cellStyle name="Note 2" xfId="420"/>
@@ -2511,10 +2609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE192"/>
+  <dimension ref="A1:AG192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2528,54 +2626,58 @@
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
     <col min="9" max="9" width="32.83203125" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.5" customWidth="1"/>
-    <col min="16" max="16" width="34" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="14" width="8.5" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" customWidth="1"/>
+    <col min="17" max="17" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="34" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="46" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46" t="s">
+      <c r="I1" s="48"/>
+      <c r="J1" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46" t="s">
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="36" t="s">
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="37" t="s">
+      <c r="S1" s="55"/>
+      <c r="AB1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="37" t="s">
+      <c r="AC1" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" s="37" t="s">
+      <c r="AD1" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="36" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2607,37 +2709,46 @@
       <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="10" t="s">
+      <c r="N2" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC2" s="37" t="s">
+      <c r="S2" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB2" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="AD2" s="37" t="s">
+      <c r="AD2" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="37" t="s">
+      <c r="AE2" s="36" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2657,7 +2768,7 @@
       <c r="I3" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="R3" s="40" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2677,7 +2788,7 @@
       <c r="I4" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="R4" s="40" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2697,10 +2808,9 @@
       <c r="I5" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="P5" s="41" t="s">
+      <c r="R5" s="40" t="s">
         <v>235</v>
       </c>
-      <c r="Q5"/>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" t="s">
@@ -2718,10 +2828,9 @@
       <c r="I6" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="P6" s="41" t="s">
+      <c r="R6" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="Q6"/>
     </row>
     <row r="7" spans="1:31">
       <c r="A7" t="s">
@@ -2739,7 +2848,7 @@
       <c r="I7" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="P7" s="41" t="s">
+      <c r="R7" s="40" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2759,7 +2868,7 @@
       <c r="I8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="42" t="s">
+      <c r="R8" s="41" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2776,13 +2885,12 @@
       <c r="D9" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="P9" s="42" t="s">
+      <c r="R9" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:31">
       <c r="A10" t="s">
@@ -2800,9 +2908,10 @@
       <c r="I10" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="41" t="s">
+      <c r="R10" s="40" t="s">
         <v>238</v>
       </c>
+      <c r="S10" s="13"/>
     </row>
     <row r="11" spans="1:31">
       <c r="A11" t="s">
@@ -2820,7 +2929,7 @@
       <c r="I11" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="P11" s="41" t="s">
+      <c r="R11" s="40" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2840,7 +2949,7 @@
       <c r="I12" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="P12" s="41" t="s">
+      <c r="R12" s="40" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2860,7 +2969,7 @@
       <c r="I13" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="P13" s="41" t="s">
+      <c r="R13" s="40" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2880,7 +2989,7 @@
       <c r="I14" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="R14" s="40" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2900,7 +3009,7 @@
       <c r="I15" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="P15" s="43" t="s">
+      <c r="R15" s="42" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2920,11 +3029,11 @@
       <c r="I16" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="P16" s="41" t="s">
+      <c r="R16" s="40" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2943,12 +3052,11 @@
       <c r="I17" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="P17" s="44" t="s">
+      <c r="R17" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="Q17"/>
-    </row>
-    <row r="18" spans="1:31">
+    </row>
+    <row r="18" spans="1:33">
       <c r="D18" s="32"/>
       <c r="H18" t="s">
         <v>85</v>
@@ -2956,12 +3064,11 @@
       <c r="I18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="P18" s="44" t="s">
+      <c r="R18" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="Q18"/>
-    </row>
-    <row r="19" spans="1:31">
+    </row>
+    <row r="19" spans="1:33">
       <c r="D19" s="32"/>
       <c r="H19" t="s">
         <v>83</v>
@@ -2969,12 +3076,11 @@
       <c r="I19" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="P19" s="44" t="s">
+      <c r="R19" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="Q19"/>
-    </row>
-    <row r="20" spans="1:31">
+    </row>
+    <row r="20" spans="1:33">
       <c r="D20" s="32"/>
       <c r="H20" t="s">
         <v>84</v>
@@ -2982,12 +3088,11 @@
       <c r="I20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="P20" s="44" t="s">
+      <c r="R20" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="Q20"/>
-    </row>
-    <row r="21" spans="1:31">
+    </row>
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -3003,12 +3108,11 @@
       <c r="I21" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="P21" s="41" t="s">
+      <c r="R21" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="Q21"/>
-    </row>
-    <row r="22" spans="1:31">
+    </row>
+    <row r="22" spans="1:33">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -3024,11 +3128,11 @@
       <c r="I22" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="P22" s="41" t="s">
+      <c r="R22" s="40" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:33">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -3042,13 +3146,13 @@
       <c r="I23" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="P23" s="41" t="s">
+      <c r="R23" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="35"/>
-    </row>
-    <row r="24" spans="1:31">
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="35"/>
+    </row>
+    <row r="24" spans="1:33">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -3064,12 +3168,11 @@
       <c r="I24" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="P24" s="41" t="s">
+      <c r="R24" s="40" t="s">
         <v>240</v>
       </c>
-      <c r="Q24"/>
-    </row>
-    <row r="25" spans="1:31">
+    </row>
+    <row r="25" spans="1:33">
       <c r="A25" t="s">
         <v>151</v>
       </c>
@@ -3082,15 +3185,14 @@
       <c r="D25" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="P25" s="41" t="s">
+      <c r="R25" s="40" t="s">
         <v>240</v>
       </c>
-      <c r="Q25"/>
-    </row>
-    <row r="26" spans="1:31">
+    </row>
+    <row r="26" spans="1:33">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3106,12 +3208,11 @@
       <c r="I26" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="P26" s="44" t="s">
+      <c r="R26" s="43" t="s">
         <v>227</v>
       </c>
-      <c r="Q26"/>
-    </row>
-    <row r="27" spans="1:31">
+    </row>
+    <row r="27" spans="1:33">
       <c r="A27" t="s">
         <v>152</v>
       </c>
@@ -3127,12 +3228,11 @@
       <c r="I27" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="P27" s="41" t="s">
+      <c r="R27" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="Q27"/>
-    </row>
-    <row r="28" spans="1:31">
+    </row>
+    <row r="28" spans="1:33">
       <c r="A28" t="s">
         <v>128</v>
       </c>
@@ -3148,12 +3248,11 @@
       <c r="I28" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="P28" s="41" t="s">
+      <c r="R28" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="Q28"/>
-    </row>
-    <row r="29" spans="1:31">
+    </row>
+    <row r="29" spans="1:33">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -3169,12 +3268,11 @@
       <c r="I29" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="P29" s="44" t="s">
+      <c r="R29" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="Q29"/>
-    </row>
-    <row r="30" spans="1:31">
+    </row>
+    <row r="30" spans="1:33">
       <c r="A30" t="s">
         <v>156</v>
       </c>
@@ -3190,12 +3288,11 @@
       <c r="I30" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="P30" s="41" t="s">
+      <c r="R30" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="Q30"/>
-    </row>
-    <row r="31" spans="1:31">
+    </row>
+    <row r="31" spans="1:33">
       <c r="A31" t="s">
         <v>157</v>
       </c>
@@ -3211,18 +3308,15 @@
       <c r="I31" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
       <c r="O31" s="12"/>
-      <c r="P31" s="41" t="s">
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
-      <c r="S31" s="12"/>
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
       <c r="V31" s="12"/>
@@ -3235,8 +3329,10 @@
       <c r="AC31" s="12"/>
       <c r="AD31" s="12"/>
       <c r="AE31" s="12"/>
-    </row>
-    <row r="32" spans="1:31">
+      <c r="AF31" s="12"/>
+      <c r="AG31" s="12"/>
+    </row>
+    <row r="32" spans="1:33">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -3252,12 +3348,11 @@
       <c r="I32" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="P32" s="41" t="s">
+      <c r="R32" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="Q32"/>
-    </row>
-    <row r="33" spans="1:17">
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -3273,12 +3368,11 @@
       <c r="I33" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="P33" s="41" t="s">
+      <c r="R33" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="Q33"/>
-    </row>
-    <row r="34" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="34" spans="1:18" ht="16" customHeight="1">
       <c r="A34" t="s">
         <v>164</v>
       </c>
@@ -3294,12 +3388,11 @@
       <c r="I34" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="P34" s="41" t="s">
+      <c r="R34" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="Q34"/>
-    </row>
-    <row r="35" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="35" spans="1:18" ht="16" customHeight="1">
       <c r="A35" t="s">
         <v>166</v>
       </c>
@@ -3315,12 +3408,11 @@
       <c r="I35" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="P35" s="41" t="s">
+      <c r="R35" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="Q35"/>
-    </row>
-    <row r="36" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="36" spans="1:18" ht="16" customHeight="1">
       <c r="A36" s="12" t="s">
         <v>167</v>
       </c>
@@ -3337,15 +3429,14 @@
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="38" t="s">
+      <c r="I36" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="P36" s="41" t="s">
+      <c r="R36" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="Q36"/>
-    </row>
-    <row r="37" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="37" spans="1:18" ht="16" customHeight="1">
       <c r="A37" t="s">
         <v>170</v>
       </c>
@@ -3359,12 +3450,11 @@
       <c r="I37" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="P37" s="41" t="s">
+      <c r="R37" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="Q37"/>
-    </row>
-    <row r="38" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="38" spans="1:18" ht="16" customHeight="1">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -3378,12 +3468,11 @@
       <c r="I38" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="P38" s="41" t="s">
+      <c r="R38" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="Q38"/>
-    </row>
-    <row r="39" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="39" spans="1:18" ht="16" customHeight="1">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -3397,12 +3486,11 @@
       <c r="I39" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="P39" s="41" t="s">
+      <c r="R39" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="Q39"/>
-    </row>
-    <row r="40" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="40" spans="1:18" ht="16" customHeight="1">
       <c r="A40" t="s">
         <v>176</v>
       </c>
@@ -3416,12 +3504,11 @@
       <c r="I40" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="P40" s="41" t="s">
+      <c r="R40" s="40" t="s">
         <v>204</v>
       </c>
-      <c r="Q40"/>
-    </row>
-    <row r="41" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="41" spans="1:18" ht="16" customHeight="1">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -3435,12 +3522,11 @@
       <c r="I41" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="P41" s="41" t="s">
+      <c r="R41" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="Q41"/>
-    </row>
-    <row r="42" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="42" spans="1:18" ht="16" customHeight="1">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -3454,12 +3540,11 @@
       <c r="I42" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="P42" s="41" t="s">
+      <c r="R42" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="Q42"/>
-    </row>
-    <row r="43" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="43" spans="1:18" ht="16" customHeight="1">
       <c r="A43" t="s">
         <v>180</v>
       </c>
@@ -3473,12 +3558,11 @@
       <c r="I43" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="P43" s="41" t="s">
+      <c r="R43" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="Q43"/>
-    </row>
-    <row r="44" spans="1:17" ht="16" customHeight="1">
+    </row>
+    <row r="44" spans="1:18" ht="16" customHeight="1">
       <c r="A44" t="s">
         <v>181</v>
       </c>
@@ -3492,12 +3576,11 @@
       <c r="I44" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="P44" s="41" t="s">
+      <c r="R44" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="Q44"/>
-    </row>
-    <row r="45" spans="1:17">
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -3511,12 +3594,11 @@
       <c r="I45" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="P45" s="41" t="s">
+      <c r="R45" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="Q45"/>
-    </row>
-    <row r="46" spans="1:17">
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -3530,12 +3612,11 @@
       <c r="I46" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="P46" s="41" t="s">
+      <c r="R46" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="Q46"/>
-    </row>
-    <row r="47" spans="1:17">
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" t="s">
         <v>190</v>
       </c>
@@ -3549,12 +3630,11 @@
       <c r="I47" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="P47" s="41" t="s">
+      <c r="R47" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="Q47"/>
-    </row>
-    <row r="48" spans="1:17">
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" t="s">
         <v>192</v>
       </c>
@@ -3568,11 +3648,11 @@
       <c r="I48" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="P48" s="41" t="s">
+      <c r="R48" s="40" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:18">
       <c r="A49" t="s">
         <v>193</v>
       </c>
@@ -3586,11 +3666,11 @@
       <c r="I49" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="P49" s="41" t="s">
+      <c r="R49" s="40" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:18">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -3606,11 +3686,11 @@
       <c r="I50" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P50" s="41" t="s">
+      <c r="R50" s="40" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:18">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -3626,12 +3706,11 @@
       <c r="I51" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="P51" s="41" t="s">
+      <c r="R51" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="Q51"/>
-    </row>
-    <row r="52" spans="1:17">
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -3647,196 +3726,164 @@
       <c r="I52" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="P52" s="41" t="s">
+      <c r="R52" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="Q52"/>
-    </row>
-    <row r="53" spans="1:17">
-      <c r="Q53"/>
-    </row>
-    <row r="54" spans="1:17">
-      <c r="Q54"/>
-    </row>
-    <row r="55" spans="1:17">
-      <c r="Q55"/>
-    </row>
-    <row r="56" spans="1:17">
+    </row>
+    <row r="56" spans="1:18">
       <c r="I56" s="9"/>
-      <c r="Q56"/>
-    </row>
-    <row r="57" spans="1:17">
+    </row>
+    <row r="57" spans="1:18">
       <c r="I57" s="9"/>
-      <c r="Q57"/>
-    </row>
-    <row r="58" spans="1:17">
+    </row>
+    <row r="58" spans="1:18">
       <c r="I58" s="9"/>
-      <c r="Q58"/>
-    </row>
-    <row r="59" spans="1:17">
+    </row>
+    <row r="59" spans="1:18">
       <c r="I59" s="9"/>
-      <c r="Q59"/>
-    </row>
-    <row r="60" spans="1:17">
+    </row>
+    <row r="60" spans="1:18">
       <c r="I60" s="9"/>
-      <c r="Q60"/>
-    </row>
-    <row r="61" spans="1:17">
+    </row>
+    <row r="61" spans="1:18">
       <c r="I61" s="9"/>
-      <c r="Q61"/>
-    </row>
-    <row r="62" spans="1:17">
+    </row>
+    <row r="62" spans="1:18">
       <c r="I62" s="9"/>
-      <c r="Q62"/>
-    </row>
-    <row r="63" spans="1:17">
+    </row>
+    <row r="63" spans="1:18">
       <c r="I63" s="9"/>
-      <c r="Q63"/>
-    </row>
-    <row r="64" spans="1:17">
+    </row>
+    <row r="64" spans="1:18">
       <c r="I64" s="9"/>
-      <c r="Q64"/>
-    </row>
-    <row r="65" spans="4:18">
+    </row>
+    <row r="65" spans="4:20">
       <c r="I65" s="9"/>
-      <c r="Q65"/>
-    </row>
-    <row r="66" spans="4:18">
+    </row>
+    <row r="66" spans="4:20">
       <c r="I66" s="9"/>
-      <c r="Q66"/>
-    </row>
-    <row r="67" spans="4:18">
+    </row>
+    <row r="67" spans="4:20">
       <c r="D67" s="9"/>
       <c r="I67" s="9"/>
-      <c r="M67" s="26"/>
-      <c r="N67" s="26"/>
-      <c r="Q67"/>
-    </row>
-    <row r="68" spans="4:18">
+      <c r="O67" s="26"/>
+      <c r="P67" s="26"/>
+    </row>
+    <row r="68" spans="4:20">
       <c r="D68" s="9"/>
       <c r="I68" s="9"/>
-      <c r="Q68"/>
-    </row>
-    <row r="69" spans="4:18">
+    </row>
+    <row r="69" spans="4:20">
       <c r="I69" s="9"/>
-      <c r="P69" s="27"/>
-      <c r="Q69"/>
-    </row>
-    <row r="70" spans="4:18">
+      <c r="R69" s="27"/>
+    </row>
+    <row r="70" spans="4:20">
       <c r="I70" s="9"/>
-      <c r="Q70"/>
-    </row>
-    <row r="71" spans="4:18">
+    </row>
+    <row r="71" spans="4:20">
       <c r="D71" s="9"/>
       <c r="I71" s="9"/>
-      <c r="Q71"/>
-    </row>
-    <row r="72" spans="4:18">
+    </row>
+    <row r="72" spans="4:20">
       <c r="D72" s="9"/>
       <c r="I72" s="9"/>
-      <c r="Q72"/>
-    </row>
-    <row r="73" spans="4:18">
+    </row>
+    <row r="73" spans="4:20">
       <c r="D73" s="9"/>
       <c r="I73" s="9"/>
-      <c r="M73" s="26"/>
-      <c r="N73" s="26"/>
-      <c r="Q73"/>
-    </row>
-    <row r="74" spans="4:18">
+      <c r="O73" s="26"/>
+      <c r="P73" s="26"/>
+    </row>
+    <row r="74" spans="4:20">
       <c r="D74" s="9"/>
       <c r="I74" s="9"/>
-      <c r="Q74"/>
-    </row>
-    <row r="75" spans="4:18">
+    </row>
+    <row r="75" spans="4:20">
       <c r="I75" s="9"/>
-      <c r="Q75"/>
-    </row>
-    <row r="76" spans="4:18">
+    </row>
+    <row r="76" spans="4:20">
       <c r="I76" s="9"/>
-      <c r="Q76"/>
-    </row>
-    <row r="77" spans="4:18">
+    </row>
+    <row r="77" spans="4:20">
       <c r="I77" s="9"/>
-      <c r="M77" s="26"/>
-      <c r="N77" s="26"/>
-      <c r="Q77"/>
-    </row>
-    <row r="78" spans="4:18">
+      <c r="O77" s="26"/>
+      <c r="P77" s="26"/>
+    </row>
+    <row r="78" spans="4:20">
       <c r="I78" s="9"/>
-      <c r="P78" s="27"/>
-    </row>
-    <row r="79" spans="4:18">
+      <c r="R78" s="27"/>
+    </row>
+    <row r="79" spans="4:20">
       <c r="I79" s="9"/>
-      <c r="P79" s="27"/>
-    </row>
-    <row r="80" spans="4:18">
+      <c r="R79" s="27"/>
+    </row>
+    <row r="80" spans="4:20">
       <c r="I80" s="9"/>
-      <c r="R80" s="17"/>
-    </row>
-    <row r="81" spans="4:30">
+      <c r="T80" s="17"/>
+    </row>
+    <row r="81" spans="4:32">
       <c r="I81" s="9"/>
     </row>
-    <row r="82" spans="4:30">
+    <row r="82" spans="4:32">
       <c r="I82" s="9"/>
-      <c r="M82" s="25"/>
-      <c r="N82" s="25"/>
-    </row>
-    <row r="83" spans="4:30">
+      <c r="O82" s="25"/>
+      <c r="P82" s="25"/>
+    </row>
+    <row r="83" spans="4:32">
       <c r="I83" s="9"/>
-      <c r="M83" s="25"/>
-      <c r="N83" s="25"/>
-    </row>
-    <row r="84" spans="4:30">
+      <c r="J83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="25"/>
+      <c r="P83" s="25"/>
+      <c r="S83" s="13"/>
+    </row>
+    <row r="84" spans="4:32">
       <c r="I84" s="9"/>
     </row>
-    <row r="85" spans="4:30">
+    <row r="85" spans="4:32">
       <c r="D85" s="9"/>
       <c r="I85" s="9"/>
     </row>
-    <row r="86" spans="4:30">
+    <row r="86" spans="4:32">
       <c r="D86" s="9"/>
       <c r="I86" s="9"/>
     </row>
-    <row r="87" spans="4:30">
+    <row r="87" spans="4:32">
       <c r="I87" s="9"/>
     </row>
-    <row r="88" spans="4:30">
+    <row r="88" spans="4:32">
       <c r="I88" s="9"/>
     </row>
-    <row r="89" spans="4:30">
+    <row r="89" spans="4:32">
       <c r="I89" s="9"/>
-      <c r="P89" s="28"/>
-    </row>
-    <row r="90" spans="4:30">
+      <c r="R89" s="28"/>
+    </row>
+    <row r="90" spans="4:32">
       <c r="I90" s="9"/>
-      <c r="P90" s="28"/>
-    </row>
-    <row r="91" spans="4:30">
+      <c r="R90" s="28"/>
+    </row>
+    <row r="91" spans="4:32">
       <c r="I91" s="9"/>
     </row>
-    <row r="92" spans="4:30">
+    <row r="92" spans="4:32">
       <c r="I92" s="9"/>
     </row>
-    <row r="93" spans="4:30">
+    <row r="93" spans="4:32">
       <c r="I93" s="9"/>
-      <c r="P93" s="6"/>
-      <c r="AB93" s="7"/>
-      <c r="AC93" s="8"/>
-      <c r="AD93" s="6"/>
-    </row>
-    <row r="94" spans="4:30">
+      <c r="R93" s="6"/>
+      <c r="AD93" s="7"/>
+      <c r="AE93" s="8"/>
+      <c r="AF93" s="6"/>
+    </row>
+    <row r="94" spans="4:32">
       <c r="I94" s="9"/>
-      <c r="J94" s="6"/>
       <c r="K94" s="6"/>
       <c r="L94" s="6"/>
       <c r="M94" s="6"/>
-      <c r="N94" s="6"/>
       <c r="O94" s="6"/>
       <c r="P94" s="6"/>
-      <c r="Q94" s="13"/>
+      <c r="Q94" s="6"/>
       <c r="R94" s="6"/>
-      <c r="S94" s="6"/>
       <c r="T94" s="6"/>
       <c r="U94" s="6"/>
       <c r="V94" s="6"/>
@@ -3845,27 +3892,29 @@
       <c r="Y94" s="6"/>
       <c r="Z94" s="6"/>
       <c r="AA94" s="6"/>
-      <c r="AB94" s="7"/>
-      <c r="AC94" s="8"/>
-      <c r="AD94" s="6"/>
-    </row>
-    <row r="95" spans="4:30">
+      <c r="AB94" s="6"/>
+      <c r="AC94" s="6"/>
+      <c r="AD94" s="7"/>
+      <c r="AE94" s="8"/>
+      <c r="AF94" s="6"/>
+    </row>
+    <row r="95" spans="4:32">
       <c r="I95" s="9"/>
-      <c r="P95" s="6"/>
-    </row>
-    <row r="96" spans="4:30">
+      <c r="R95" s="6"/>
+    </row>
+    <row r="96" spans="4:32">
       <c r="D96" s="9"/>
       <c r="I96" s="9"/>
-      <c r="P96" s="6"/>
-    </row>
-    <row r="97" spans="1:18">
+      <c r="R96" s="6"/>
+    </row>
+    <row r="97" spans="1:20">
       <c r="D97" s="9"/>
       <c r="I97" s="9"/>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:20">
       <c r="I98" s="9"/>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:20">
       <c r="A99" s="19"/>
       <c r="B99" s="20"/>
       <c r="C99" s="6"/>
@@ -3876,315 +3925,299 @@
       <c r="H99" s="6"/>
       <c r="I99" s="24"/>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:20">
       <c r="I100" s="9"/>
-      <c r="R100" s="17"/>
-    </row>
-    <row r="101" spans="1:18">
+      <c r="S100" s="13"/>
+      <c r="T100" s="17"/>
+    </row>
+    <row r="101" spans="1:20">
       <c r="I101" s="9"/>
-    </row>
-    <row r="102" spans="1:18">
+      <c r="S101" s="29"/>
+    </row>
+    <row r="102" spans="1:20">
       <c r="I102" s="9"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:20">
       <c r="I103" s="9"/>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:20">
       <c r="I104" s="9"/>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:20">
       <c r="D105" s="9"/>
       <c r="I105" s="9"/>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:20">
       <c r="I106" s="9"/>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:20">
       <c r="I107" s="9"/>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:20">
       <c r="I108" s="9"/>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:20">
       <c r="I109" s="9"/>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:20">
       <c r="I110" s="9"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:20">
       <c r="I111" s="9"/>
-      <c r="Q111" s="13"/>
-    </row>
-    <row r="112" spans="1:18">
+    </row>
+    <row r="112" spans="1:20">
       <c r="I112" s="9"/>
-      <c r="P112" s="28"/>
-      <c r="Q112" s="29"/>
-    </row>
-    <row r="113" spans="4:17">
+      <c r="R112" s="28"/>
+    </row>
+    <row r="113" spans="4:19">
       <c r="I113" s="9"/>
     </row>
-    <row r="114" spans="4:17">
+    <row r="114" spans="4:19">
       <c r="I114" s="9"/>
     </row>
-    <row r="115" spans="4:17">
+    <row r="115" spans="4:19">
       <c r="I115" s="9"/>
     </row>
-    <row r="116" spans="4:17">
+    <row r="116" spans="4:19">
       <c r="D116" s="9"/>
       <c r="I116" s="11"/>
-    </row>
-    <row r="117" spans="4:17">
+      <c r="S116" s="14"/>
+    </row>
+    <row r="117" spans="4:19">
       <c r="I117" s="9"/>
-    </row>
-    <row r="118" spans="4:17">
+      <c r="S117" s="14"/>
+    </row>
+    <row r="118" spans="4:19">
       <c r="D118" s="9"/>
       <c r="I118" s="9"/>
-    </row>
-    <row r="119" spans="4:17">
+      <c r="S118" s="13"/>
+    </row>
+    <row r="119" spans="4:19">
       <c r="I119" s="9"/>
     </row>
-    <row r="120" spans="4:17">
+    <row r="120" spans="4:19">
       <c r="I120" s="9"/>
-      <c r="M120" s="25"/>
-      <c r="N120" s="25"/>
-    </row>
-    <row r="121" spans="4:17">
+      <c r="O120" s="25"/>
+      <c r="P120" s="25"/>
+    </row>
+    <row r="121" spans="4:19">
       <c r="I121" s="9"/>
-    </row>
-    <row r="122" spans="4:17">
+      <c r="S121" s="13"/>
+    </row>
+    <row r="122" spans="4:19">
       <c r="I122" s="9"/>
-    </row>
-    <row r="123" spans="4:17">
+      <c r="S122" s="13"/>
+    </row>
+    <row r="123" spans="4:19">
       <c r="I123" s="9"/>
-    </row>
-    <row r="124" spans="4:17">
+      <c r="S123" s="13"/>
+    </row>
+    <row r="124" spans="4:19">
       <c r="I124" s="9"/>
-    </row>
-    <row r="125" spans="4:17">
+      <c r="S124" s="29"/>
+    </row>
+    <row r="125" spans="4:19">
       <c r="I125" s="9"/>
-    </row>
-    <row r="126" spans="4:17">
+      <c r="S125" s="29"/>
+    </row>
+    <row r="126" spans="4:19">
       <c r="I126" s="9"/>
-    </row>
-    <row r="127" spans="4:17">
+      <c r="S126" s="14"/>
+    </row>
+    <row r="127" spans="4:19">
       <c r="I127" s="9"/>
-      <c r="Q127" s="14"/>
-    </row>
-    <row r="128" spans="4:17">
+      <c r="S127" s="14"/>
+    </row>
+    <row r="128" spans="4:19">
       <c r="D128" s="9"/>
       <c r="I128" s="9"/>
-      <c r="Q128" s="14"/>
-    </row>
-    <row r="129" spans="4:17">
+      <c r="S128" s="13"/>
+    </row>
+    <row r="129" spans="4:19">
       <c r="D129" s="9"/>
       <c r="I129" s="9"/>
-      <c r="Q129" s="13"/>
-    </row>
-    <row r="130" spans="4:17">
+      <c r="S129" s="13"/>
+    </row>
+    <row r="130" spans="4:19">
       <c r="D130" s="9"/>
       <c r="I130" s="9"/>
     </row>
-    <row r="131" spans="4:17">
+    <row r="131" spans="4:19">
       <c r="D131" s="9"/>
       <c r="I131" s="9"/>
     </row>
-    <row r="132" spans="4:17">
+    <row r="132" spans="4:19">
       <c r="I132" s="9"/>
-      <c r="Q132" s="13"/>
-    </row>
-    <row r="133" spans="4:17">
+    </row>
+    <row r="133" spans="4:19">
       <c r="I133" s="9"/>
-      <c r="Q133" s="13"/>
-    </row>
-    <row r="134" spans="4:17">
+    </row>
+    <row r="134" spans="4:19">
       <c r="I134" s="9"/>
-      <c r="Q134" s="13"/>
-    </row>
-    <row r="135" spans="4:17">
+    </row>
+    <row r="135" spans="4:19">
       <c r="I135" s="9"/>
-      <c r="P135" s="28"/>
-      <c r="Q135" s="29"/>
-    </row>
-    <row r="136" spans="4:17">
+      <c r="R135" s="28"/>
+    </row>
+    <row r="136" spans="4:19">
       <c r="I136" s="9"/>
-      <c r="P136" s="28"/>
-      <c r="Q136" s="29"/>
-    </row>
-    <row r="137" spans="4:17">
+      <c r="R136" s="28"/>
+    </row>
+    <row r="137" spans="4:19">
       <c r="I137" s="9"/>
-      <c r="Q137" s="14"/>
-    </row>
-    <row r="138" spans="4:17">
+    </row>
+    <row r="138" spans="4:19">
       <c r="I138" s="9"/>
-      <c r="Q138" s="14"/>
-    </row>
-    <row r="139" spans="4:17">
+    </row>
+    <row r="139" spans="4:19">
       <c r="I139" s="9"/>
-      <c r="Q139" s="13"/>
-    </row>
-    <row r="140" spans="4:17">
+    </row>
+    <row r="140" spans="4:19">
       <c r="I140" s="22"/>
-      <c r="Q140" s="13"/>
-    </row>
-    <row r="141" spans="4:17">
+    </row>
+    <row r="141" spans="4:19">
       <c r="I141" s="22"/>
     </row>
-    <row r="142" spans="4:17">
+    <row r="142" spans="4:19">
       <c r="D142" s="9"/>
       <c r="I142" s="9"/>
-      <c r="Q142"/>
-    </row>
-    <row r="143" spans="4:17">
+    </row>
+    <row r="143" spans="4:19">
       <c r="D143" s="9"/>
       <c r="I143" s="9"/>
-      <c r="Q143"/>
-    </row>
-    <row r="144" spans="4:17">
+    </row>
+    <row r="144" spans="4:19">
       <c r="D144" s="9"/>
       <c r="I144" s="11"/>
-      <c r="Q144"/>
-    </row>
-    <row r="145" spans="4:17">
+    </row>
+    <row r="145" spans="4:18">
       <c r="D145" s="9"/>
       <c r="I145" s="11"/>
-      <c r="Q145"/>
-    </row>
-    <row r="146" spans="4:17">
+    </row>
+    <row r="146" spans="4:18">
       <c r="D146" s="9"/>
       <c r="I146" s="9"/>
-      <c r="Q146"/>
-    </row>
-    <row r="147" spans="4:17">
+    </row>
+    <row r="147" spans="4:18">
       <c r="D147" s="9"/>
       <c r="I147" s="9"/>
-      <c r="Q147"/>
-    </row>
-    <row r="148" spans="4:17">
+    </row>
+    <row r="148" spans="4:18">
       <c r="D148" s="9"/>
       <c r="I148" s="9"/>
-      <c r="Q148"/>
-    </row>
-    <row r="149" spans="4:17">
+    </row>
+    <row r="149" spans="4:18">
       <c r="D149" s="9"/>
       <c r="I149" s="9"/>
-      <c r="Q149"/>
-    </row>
-    <row r="150" spans="4:17">
+    </row>
+    <row r="150" spans="4:18">
       <c r="I150" s="9"/>
-      <c r="P150" s="12"/>
-      <c r="Q150"/>
-    </row>
-    <row r="151" spans="4:17">
+      <c r="R150" s="12"/>
+    </row>
+    <row r="151" spans="4:18">
       <c r="I151" s="9"/>
-      <c r="P151" s="12"/>
-      <c r="Q151"/>
-    </row>
-    <row r="152" spans="4:17">
+      <c r="R151" s="12"/>
+    </row>
+    <row r="152" spans="4:18">
       <c r="I152" s="9"/>
-      <c r="P152" s="12"/>
-      <c r="Q152"/>
-    </row>
-    <row r="153" spans="4:17">
+      <c r="R152" s="12"/>
+    </row>
+    <row r="153" spans="4:18">
       <c r="I153" s="9"/>
-      <c r="P153" s="12"/>
-      <c r="Q153"/>
-    </row>
-    <row r="154" spans="4:17">
+      <c r="R153" s="12"/>
+    </row>
+    <row r="154" spans="4:18">
       <c r="I154" s="9"/>
-      <c r="P154" s="12"/>
-      <c r="Q154"/>
-    </row>
-    <row r="155" spans="4:17">
+      <c r="R154" s="12"/>
+    </row>
+    <row r="155" spans="4:18">
       <c r="I155" s="9"/>
-      <c r="Q155"/>
-    </row>
-    <row r="156" spans="4:17">
+    </row>
+    <row r="156" spans="4:18">
       <c r="I156" s="9"/>
-      <c r="Q156"/>
-    </row>
-    <row r="157" spans="4:17">
+    </row>
+    <row r="157" spans="4:18">
       <c r="I157" s="9"/>
-      <c r="P157" s="15"/>
-      <c r="Q157"/>
-    </row>
-    <row r="158" spans="4:17">
+      <c r="R157" s="15"/>
+    </row>
+    <row r="158" spans="4:18">
       <c r="I158" s="9"/>
-      <c r="P158" s="15"/>
-    </row>
-    <row r="159" spans="4:17">
+      <c r="R158" s="15"/>
+    </row>
+    <row r="159" spans="4:18">
       <c r="I159" s="9"/>
     </row>
-    <row r="160" spans="4:17">
+    <row r="160" spans="4:18">
       <c r="D160" s="9"/>
       <c r="I160" s="9"/>
     </row>
-    <row r="161" spans="4:18">
+    <row r="161" spans="4:20">
       <c r="D161" s="9"/>
       <c r="I161" s="9"/>
     </row>
-    <row r="162" spans="4:18">
+    <row r="162" spans="4:20">
       <c r="I162" s="9"/>
     </row>
-    <row r="163" spans="4:18">
+    <row r="163" spans="4:20">
       <c r="I163" s="9"/>
     </row>
-    <row r="164" spans="4:18">
+    <row r="164" spans="4:20">
       <c r="D164" s="9"/>
       <c r="I164" s="9"/>
-      <c r="R164" s="17"/>
-    </row>
-    <row r="165" spans="4:18">
+      <c r="T164" s="17"/>
+    </row>
+    <row r="165" spans="4:20">
       <c r="D165" s="9"/>
       <c r="I165" s="9"/>
     </row>
-    <row r="166" spans="4:18">
+    <row r="166" spans="4:20">
       <c r="D166" s="9"/>
       <c r="I166" s="9"/>
-      <c r="P166" s="27"/>
-    </row>
-    <row r="167" spans="4:18">
+      <c r="R166" s="27"/>
+    </row>
+    <row r="167" spans="4:20">
       <c r="D167" s="9"/>
       <c r="I167" s="9"/>
     </row>
-    <row r="168" spans="4:18">
+    <row r="168" spans="4:20">
       <c r="D168" s="9"/>
       <c r="I168" s="9"/>
     </row>
-    <row r="169" spans="4:18">
+    <row r="169" spans="4:20">
       <c r="D169" s="9"/>
       <c r="I169" s="9"/>
     </row>
-    <row r="170" spans="4:18">
+    <row r="170" spans="4:20">
       <c r="D170" s="9"/>
       <c r="I170" s="9"/>
     </row>
-    <row r="171" spans="4:18">
+    <row r="171" spans="4:20">
       <c r="D171" s="9"/>
       <c r="I171" s="9"/>
     </row>
-    <row r="172" spans="4:18">
+    <row r="172" spans="4:20">
       <c r="I172" s="9"/>
     </row>
-    <row r="173" spans="4:18">
+    <row r="173" spans="4:20">
       <c r="I173" s="9"/>
     </row>
-    <row r="174" spans="4:18">
+    <row r="174" spans="4:20">
       <c r="I174" s="9"/>
     </row>
-    <row r="175" spans="4:18">
+    <row r="175" spans="4:20">
       <c r="I175" s="9"/>
     </row>
-    <row r="176" spans="4:18">
+    <row r="176" spans="4:20">
       <c r="I176" s="9"/>
     </row>
-    <row r="177" spans="1:30">
+    <row r="177" spans="1:32">
       <c r="I177" s="9"/>
-      <c r="P177" s="28"/>
-    </row>
-    <row r="178" spans="1:30">
+      <c r="R177" s="28"/>
+    </row>
+    <row r="178" spans="1:32">
       <c r="I178" s="9"/>
     </row>
-    <row r="179" spans="1:30" s="16" customFormat="1">
+    <row r="179" spans="1:32" s="16" customFormat="1">
       <c r="A179"/>
       <c r="B179"/>
       <c r="C179"/>
@@ -4201,9 +4234,9 @@
       <c r="N179"/>
       <c r="O179"/>
       <c r="P179"/>
-      <c r="Q179" s="1"/>
+      <c r="Q179"/>
       <c r="R179"/>
-      <c r="S179"/>
+      <c r="S179" s="1"/>
       <c r="T179"/>
       <c r="U179"/>
       <c r="V179"/>
@@ -4215,71 +4248,71 @@
       <c r="AB179"/>
       <c r="AC179"/>
       <c r="AD179"/>
-    </row>
-    <row r="180" spans="1:30">
+      <c r="AE179"/>
+      <c r="AF179"/>
+    </row>
+    <row r="180" spans="1:32">
       <c r="I180" s="9"/>
     </row>
-    <row r="181" spans="1:30">
+    <row r="181" spans="1:32">
       <c r="I181" s="9"/>
-      <c r="P181" s="27"/>
-    </row>
-    <row r="182" spans="1:30">
+      <c r="R181" s="27"/>
+    </row>
+    <row r="182" spans="1:32">
       <c r="I182" s="9"/>
     </row>
-    <row r="183" spans="1:30">
+    <row r="183" spans="1:32">
       <c r="D183" s="9"/>
       <c r="I183" s="9"/>
     </row>
-    <row r="186" spans="1:30">
+    <row r="186" spans="1:32">
       <c r="I186" s="9"/>
     </row>
-    <row r="187" spans="1:30">
+    <row r="187" spans="1:32">
       <c r="D187" s="9"/>
       <c r="I187" s="23"/>
     </row>
-    <row r="188" spans="1:30">
+    <row r="188" spans="1:32">
       <c r="I188" s="23"/>
     </row>
-    <row r="189" spans="1:30">
+    <row r="189" spans="1:32">
       <c r="I189" s="23"/>
     </row>
-    <row r="190" spans="1:30">
+    <row r="190" spans="1:32">
       <c r="D190" s="9"/>
       <c r="I190" s="9"/>
     </row>
-    <row r="191" spans="1:30">
+    <row r="191" spans="1:32">
       <c r="I191" s="9"/>
     </row>
-    <row r="192" spans="1:30">
+    <row r="192" spans="1:32">
       <c r="D192" s="9"/>
       <c r="I192" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="R1:S1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:B68 B8:B35">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53:B68">
       <formula1>$AB$1:$AE$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C144:C154 C56:C142 C159:C192 C37:C52 C8:C35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C144:C154 C8:C35 C159:C192 C37:C142">
       <formula1>$AB$2:$AE$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B144:B154 B69:B142 B159:B192">
-      <formula1>$AB$1:$AB$47</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B7">
-      <formula1>$AB$1:$AB$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B144:B154 B159:B192 B69:B142">
+      <formula1>$AD$1:$AD$47</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C7">
-      <formula1>$AC$1:$AC$3</formula1>
+      <formula1>AB$2:AE$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>AB2:AB4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B52">
+      <formula1>AB$1:AE$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4321,44 +4354,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="46" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46" t="s">
+      <c r="I1" s="48"/>
+      <c r="J1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="45" t="s">
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="37" t="s">
+      <c r="AB1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="37" t="s">
+      <c r="AC1" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" s="37" t="s">
+      <c r="AD1" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="36" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4372,19 +4405,19 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="45" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -4396,13 +4429,13 @@
       <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="45" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="45" t="s">
         <v>17</v>
       </c>
       <c r="O2" s="10" t="s">
@@ -4411,16 +4444,16 @@
       <c r="P2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC2" s="37" t="s">
+      <c r="AB2" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="AD2" s="37" t="s">
+      <c r="AD2" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="37" t="s">
+      <c r="AE2" s="36" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4544,7 +4577,7 @@
       <c r="D9" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="38" t="s">
         <v>146</v>
       </c>
       <c r="P9" s="28" t="s">
@@ -4838,7 +4871,7 @@
       <c r="D25" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="39" t="s">
         <v>200</v>
       </c>
       <c r="Q25"/>
@@ -5072,7 +5105,7 @@
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="38" t="s">
+      <c r="I36" s="37" t="s">
         <v>169</v>
       </c>
       <c r="P36" s="12"/>
@@ -5473,13 +5506,13 @@
     </row>
     <row r="82" spans="4:30">
       <c r="I82" s="9"/>
-      <c r="M82" s="51"/>
-      <c r="N82" s="51"/>
+      <c r="M82" s="46"/>
+      <c r="N82" s="46"/>
     </row>
     <row r="83" spans="4:30">
       <c r="I83" s="9"/>
-      <c r="M83" s="51"/>
-      <c r="N83" s="51"/>
+      <c r="M83" s="46"/>
+      <c r="N83" s="46"/>
     </row>
     <row r="84" spans="4:30">
       <c r="I84" s="9"/>
@@ -5639,8 +5672,8 @@
     </row>
     <row r="120" spans="4:17">
       <c r="I120" s="9"/>
-      <c r="M120" s="51"/>
-      <c r="N120" s="51"/>
+      <c r="M120" s="46"/>
+      <c r="N120" s="46"/>
     </row>
     <row r="121" spans="4:17">
       <c r="I121" s="9"/>
@@ -5717,11 +5750,11 @@
       <c r="Q139" s="13"/>
     </row>
     <row r="140" spans="4:17">
-      <c r="I140" s="52"/>
+      <c r="I140" s="47"/>
       <c r="Q140" s="13"/>
     </row>
     <row r="141" spans="4:17">
-      <c r="I141" s="52"/>
+      <c r="I141" s="47"/>
     </row>
     <row r="142" spans="4:17">
       <c r="D142" s="9"/>
@@ -5946,7 +5979,7 @@
     </row>
     <row r="192" spans="1:30">
       <c r="D192" s="9"/>
-      <c r="I192" s="52"/>
+      <c r="I192" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6015,31 +6048,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="46" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46" t="s">
+      <c r="I1" s="48"/>
+      <c r="J1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
       <c r="P1" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>